<commit_message>
261224 Finished Purchase management
</commit_message>
<xml_diff>
--- a/Daily Activity/2024 Work Sheet.xlsx
+++ b/Daily Activity/2024 Work Sheet.xlsx
@@ -15,6 +15,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Dec-12'!$A$1:$V$33</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Nov-11'!$A$1:$U$31</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="117">
   <si>
     <t xml:space="preserve">DATE</t>
   </si>
@@ -346,6 +347,18 @@
     <t xml:space="preserve">Prepared CheckList For UAT</t>
   </si>
   <si>
+    <t xml:space="preserve">Purchase KT Document Assigned(5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HQOW/ ROW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS 8182/ 8181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales Test Cycle document Assigned(8)</t>
+  </si>
+  <si>
     <t xml:space="preserve">MONTH</t>
   </si>
   <si>
@@ -401,11 +414,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="166" formatCode="hh:mm:ss"/>
-    <numFmt numFmtId="167" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="167" formatCode="hh:mm:ss"/>
+    <numFmt numFmtId="168" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -468,7 +482,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -491,6 +505,20 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -523,7 +551,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -552,11 +580,59 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -568,23 +644,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -684,6 +760,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -697,7 +777,7 @@
       <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.3"/>
@@ -1038,12 +1118,12 @@
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+      <selection pane="bottomLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="22.88"/>
@@ -1054,16 +1134,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="6" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="21.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="7.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="7.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="25.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="19.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="9.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="27.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.68"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1163,13 +1242,16 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+    <row r="4" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="n">
         <v>45599</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="8" t="s">
         <v>27</v>
       </c>
+      <c r="C4" s="8"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
@@ -1300,13 +1382,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+    <row r="11" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="n">
         <v>45606</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="8" t="s">
         <v>27</v>
       </c>
+      <c r="C11" s="8"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
@@ -1446,13 +1531,16 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+    <row r="18" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="n">
         <v>45613</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="8" t="s">
         <v>27</v>
       </c>
+      <c r="C18" s="8"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="n">
@@ -1572,27 +1660,33 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="n">
+    <row r="24" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="11" t="n">
         <v>45619</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="n">
+      <c r="C24" s="12"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="15" t="n">
         <v>45620</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="16" t="s">
         <v>27</v>
       </c>
+      <c r="C25" s="16"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="n">
         <v>45621</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="19" t="s">
         <v>57</v>
       </c>
       <c r="F26" s="0" t="s">
@@ -1715,15 +1809,19 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="n">
+    <row r="31" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7" t="n">
         <v>45626</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="8" t="s">
         <v>27</v>
       </c>
+      <c r="C31" s="8"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:U31"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1731,6 +1829,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1741,21 +1840,21 @@
   </sheetPr>
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B10" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="topRight" activeCell="D28" activeCellId="0" sqref="D28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B19" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topRight" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="22.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="22.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.58"/>
@@ -1764,9 +1863,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="21.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="15.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="7.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="25.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="18.69"/>
@@ -1841,14 +1939,14 @@
       </c>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="n">
+    <row r="2" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="20" t="n">
         <v>45627</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="21"/>
     </row>
     <row r="3" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
@@ -2021,14 +2119,14 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="n">
+    <row r="9" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="20" t="n">
         <v>45634</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="21"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
@@ -2174,15 +2272,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="n">
+    <row r="16" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="20" t="n">
         <v>45641</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="G16" s="10"/>
+      <c r="C16" s="21"/>
+      <c r="G16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="n">
@@ -2310,14 +2408,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="n">
+    <row r="23" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="20" t="n">
         <v>45648</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="9"/>
+      <c r="C23" s="21"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="n">
@@ -2326,7 +2424,7 @@
       <c r="D24" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="2" t="s">
         <v>95</v>
       </c>
       <c r="F24" s="0" t="s">
@@ -2338,7 +2436,7 @@
       <c r="H24" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="Q24" s="12" t="n">
+      <c r="Q24" s="23" t="n">
         <v>0.353472222222222</v>
       </c>
     </row>
@@ -2346,16 +2444,47 @@
       <c r="A25" s="3" t="n">
         <v>45650</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="n">
+      <c r="D25" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q25" s="23" t="n">
+        <v>0.361111111111111</v>
+      </c>
+    </row>
+    <row r="26" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="n">
         <v>45651</v>
       </c>
+      <c r="B26" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="n">
         <v>45652</v>
       </c>
+      <c r="D27" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q27" s="23" t="n">
+        <v>0.352083333333333</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="n">
@@ -2367,14 +2496,14 @@
         <v>45654</v>
       </c>
     </row>
-    <row r="30" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="n">
+    <row r="30" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="20" t="n">
         <v>45655</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="9"/>
+      <c r="C30" s="21"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="n">
@@ -2387,8 +2516,8 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
       <c r="G33" s="6"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -2419,70 +2548,70 @@
       <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>99</v>
+    <row r="1" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">COUNTIF('Oct-10'!J2:J32,"YES")</f>
@@ -2495,13 +2624,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">COUNTIF('Nov-11'!B2:B31,"YES")</f>
         <v>6</v>
       </c>
-      <c r="C12" s="15" t="n">
+      <c r="C12" s="27" t="n">
         <f aca="false">COUNTIF('Nov-11'!C2:C32,"YES")</f>
         <v>1</v>
       </c>
@@ -2512,11 +2641,11 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="B13" s="15" t="n">
+        <v>115</v>
+      </c>
+      <c r="B13" s="27" t="n">
         <f aca="false">COUNTIF('Dec-12'!B2:B31,"YES")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">COUNTIF('Dec-12'!C2:C32,"YES")</f>
@@ -2527,19 +2656,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="B15" s="16" t="n">
+    <row r="15" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="28" t="n">
         <f aca="false">SUM(B2:B13)</f>
-        <v>13</v>
-      </c>
-      <c r="C15" s="16" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" s="28" t="n">
         <f aca="false">SUM(C2:C13)</f>
         <v>1</v>
       </c>
-      <c r="D15" s="16" t="n">
+      <c r="D15" s="28" t="n">
         <f aca="false">SUM(D2:D13)</f>
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
completed sales order KT document
</commit_message>
<xml_diff>
--- a/Daily Activity/2024 Work Sheet.xlsx
+++ b/Daily Activity/2024 Work Sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="121">
   <si>
     <t xml:space="preserve">DATE</t>
   </si>
@@ -360,6 +360,15 @@
   </si>
   <si>
     <t xml:space="preserve">Sales Test Cycle document Assigned(8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inprogress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inventory test cycle (5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centra </t>
   </si>
   <si>
     <t xml:space="preserve">MONTH</t>
@@ -775,7 +784,7 @@
       <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.3"/>
@@ -1121,7 +1130,7 @@
       <selection pane="bottomLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="22.88"/>
@@ -1838,13 +1847,13 @@
   </sheetPr>
   <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B16" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
-      <selection pane="topRight" activeCell="I24" activeCellId="0" sqref="I24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B13" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topRight" activeCell="I31" activeCellId="0" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="22.88"/>
@@ -2489,7 +2498,7 @@
       <c r="E27" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="F27" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G27" s="0" t="s">
@@ -2509,11 +2518,33 @@
       <c r="A28" s="3" t="n">
         <v>45653</v>
       </c>
+      <c r="D28" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="n">
         <v>45654</v>
       </c>
+      <c r="B29" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="23"/>
     </row>
     <row r="30" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="n">
@@ -2527,6 +2558,24 @@
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="n">
         <v>45656</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2567,70 +2616,70 @@
       <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="25" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">COUNTIF('Oct-10'!J2:J32,"YES")</f>
@@ -2643,7 +2692,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">COUNTIF('Nov-11'!B2:B31,"YES")</f>
@@ -2660,11 +2709,11 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B13" s="26" t="n">
         <f aca="false">COUNTIF('Dec-12'!B2:B31,"YES")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">COUNTIF('Dec-12'!C2:C32,"YES")</f>
@@ -2677,11 +2726,11 @@
     </row>
     <row r="15" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="27" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B15" s="27" t="n">
         <f aca="false">SUM(B2:B13)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" s="27" t="n">
         <f aca="false">SUM(C2:C13)</f>

</xml_diff>

<commit_message>
311224 EOD inventoy KT document ompleted
</commit_message>
<xml_diff>
--- a/Daily Activity/2024 Work Sheet.xlsx
+++ b/Daily Activity/2024 Work Sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="122">
   <si>
     <t xml:space="preserve">DATE</t>
   </si>
@@ -369,6 +369,9 @@
   </si>
   <si>
     <t xml:space="preserve">Centra </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inventory Test Cycle document Assigned(5)</t>
   </si>
   <si>
     <t xml:space="preserve">MONTH</t>
@@ -784,7 +787,7 @@
       <selection pane="bottomLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.3"/>
@@ -1130,7 +1133,7 @@
       <selection pane="bottomLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="22.88"/>
@@ -1847,13 +1850,13 @@
   </sheetPr>
   <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B13" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
-      <selection pane="topRight" activeCell="I31" activeCellId="0" sqref="I31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="22.88"/>
@@ -2521,7 +2524,7 @@
       <c r="D28" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="2" t="s">
         <v>100</v>
       </c>
       <c r="F28" s="0" t="s">
@@ -2544,7 +2547,7 @@
       <c r="B29" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="23"/>
+      <c r="D29" s="2"/>
     </row>
     <row r="30" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="n">
@@ -2559,7 +2562,7 @@
       <c r="A31" s="3" t="n">
         <v>45656</v>
       </c>
-      <c r="D31" s="23" t="s">
+      <c r="D31" s="2" t="s">
         <v>100</v>
       </c>
       <c r="E31" s="0" t="s">
@@ -2575,12 +2578,30 @@
         <v>101</v>
       </c>
       <c r="I31" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="n">
         <v>45657</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2616,70 +2637,70 @@
       <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="25" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">COUNTIF('Oct-10'!J2:J32,"YES")</f>
@@ -2692,7 +2713,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">COUNTIF('Nov-11'!B2:B31,"YES")</f>
@@ -2709,7 +2730,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B13" s="26" t="n">
         <f aca="false">COUNTIF('Dec-12'!B2:B31,"YES")</f>
@@ -2726,7 +2747,7 @@
     </row>
     <row r="15" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="27" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B15" s="27" t="n">
         <f aca="false">SUM(B2:B13)</f>

</xml_diff>